<commit_message>
fix set cold mode wind error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -20,7 +20,7 @@
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-564314.o</t>
+    <t>lto-llvm-8eda70.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -261,7 +261,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-564314.o</c:v>
+                  <c:v>lto-llvm-8eda70.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -368,7 +368,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-564314.o</c:v>
+                  <c:v>lto-llvm-8eda70.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mc_w.l</c:v>
@@ -500,124 +500,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>89.50723266601563</c:v>
+                  <c:v>89.52720642089844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.883343696594238</c:v>
+                  <c:v>2.877853393554688</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.447590351104736</c:v>
+                  <c:v>2.442929744720459</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.144080400466919</c:v>
+                  <c:v>2.139997720718384</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.437921404838562</c:v>
+                  <c:v>0.4370875358581543</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3620439171791077</c:v>
+                  <c:v>0.3613545298576355</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2471437603235245</c:v>
+                  <c:v>0.2466731518507004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2406399697065353</c:v>
+                  <c:v>0.2401817589998245</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2016172707080841</c:v>
+                  <c:v>0.201233372092247</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1907776296138763</c:v>
+                  <c:v>0.1904143691062927</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1344115138053894</c:v>
+                  <c:v>0.1341555714607239</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.119236022233963</c:v>
+                  <c:v>0.119008980691433</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1083963811397553</c:v>
+                  <c:v>0.1081899851560593</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1062284559011459</c:v>
+                  <c:v>0.1060261800885201</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0672057569026947</c:v>
+                  <c:v>0.06707778573036194</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05419819056987763</c:v>
+                  <c:v>0.05409499257802963</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05419819056987763</c:v>
+                  <c:v>0.05409499257802963</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05203026533126831</c:v>
+                  <c:v>0.05193119123578072</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05203026533126831</c:v>
+                  <c:v>0.05193119123578072</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04769440740346909</c:v>
+                  <c:v>0.04760359227657318</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04335855320096016</c:v>
+                  <c:v>0.04327599331736565</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03902269899845123</c:v>
+                  <c:v>0.03894839435815811</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03902269899845123</c:v>
+                  <c:v>0.03894839435815811</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03902269899845123</c:v>
+                  <c:v>0.03894839435815811</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03902269899845123</c:v>
+                  <c:v>0.03894839435815811</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03685477003455162</c:v>
+                  <c:v>0.0367845930159092</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03468684107065201</c:v>
+                  <c:v>0.03462079539895058</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03251891583204269</c:v>
+                  <c:v>0.03245699405670166</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03251891583204269</c:v>
+                  <c:v>0.03245699405670166</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03035098686814308</c:v>
+                  <c:v>0.03029319457709789</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03035098686814308</c:v>
+                  <c:v>0.03029319457709789</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03035098686814308</c:v>
+                  <c:v>0.03029319457709789</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03035098686814308</c:v>
+                  <c:v>0.03029319457709789</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02818305976688862</c:v>
+                  <c:v>0.02812939509749413</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.01951134949922562</c:v>
+                  <c:v>0.01947419717907906</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01083963830024004</c:v>
+                  <c:v>0.01081899832934141</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.008671710267663002</c:v>
+                  <c:v>0.008655198849737644</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.008671710267663002</c:v>
+                  <c:v>0.008655198849737644</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.004335855133831501</c:v>
+                  <c:v>0.004327599424868822</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.004335855133831501</c:v>
+                  <c:v>0.004327599424868822</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -1093,10 +1093,10 @@
         <v>5420</v>
       </c>
       <c r="D3" s="1">
-        <v>82574</v>
+        <v>82750</v>
       </c>
       <c r="E3" s="1">
-        <v>82324</v>
+        <v>82500</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1275,16 +1275,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.50723266601563</v>
+        <v>89.52720642089844</v>
       </c>
       <c r="C3" s="1">
-        <v>82574</v>
+        <v>82750</v>
       </c>
       <c r="D3" s="1">
         <v>5420</v>
       </c>
       <c r="E3" s="1">
-        <v>82324</v>
+        <v>82500</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.883343696594238</v>
+        <v>2.877853393554688</v>
       </c>
       <c r="C4" s="1">
         <v>2660</v>
@@ -1327,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2.447590351104736</v>
+        <v>2.442929744720459</v>
       </c>
       <c r="C5" s="1">
         <v>2258</v>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2.144080400466919</v>
+        <v>2.139997720718384</v>
       </c>
       <c r="C6" s="1">
         <v>1978</v>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.437921404838562</v>
+        <v>0.4370875358581543</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3620439171791077</v>
+        <v>0.3613545298576355</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1431,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2471437603235245</v>
+        <v>0.2466731518507004</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1457,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2406399697065353</v>
+        <v>0.2401817589998245</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.2016172707080841</v>
+        <v>0.201233372092247</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1907776296138763</v>
+        <v>0.1904143691062927</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1344115138053894</v>
+        <v>0.1341555714607239</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.119236022233963</v>
+        <v>0.119008980691433</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1083963811397553</v>
+        <v>0.1081899851560593</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1613,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1062284559011459</v>
+        <v>0.1060261800885201</v>
       </c>
       <c r="C16" s="1">
         <v>98</v>
@@ -1639,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.0672057569026947</v>
+        <v>0.06707778573036194</v>
       </c>
       <c r="C17" s="1">
         <v>62</v>
@@ -1665,7 +1665,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.05419819056987763</v>
+        <v>0.05409499257802963</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1691,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.05419819056987763</v>
+        <v>0.05409499257802963</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -1717,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.05203026533126831</v>
+        <v>0.05193119123578072</v>
       </c>
       <c r="C20" s="1">
         <v>48</v>
@@ -1743,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.05203026533126831</v>
+        <v>0.05193119123578072</v>
       </c>
       <c r="C21" s="1">
         <v>48</v>
@@ -1769,7 +1769,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04769440740346909</v>
+        <v>0.04760359227657318</v>
       </c>
       <c r="C22" s="1">
         <v>44</v>
@@ -1795,7 +1795,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04335855320096016</v>
+        <v>0.04327599331736565</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
@@ -1821,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.03902269899845123</v>
+        <v>0.03894839435815811</v>
       </c>
       <c r="C24" s="1">
         <v>36</v>
@@ -1847,7 +1847,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03902269899845123</v>
+        <v>0.03894839435815811</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1873,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03902269899845123</v>
+        <v>0.03894839435815811</v>
       </c>
       <c r="C26" s="1">
         <v>36</v>
@@ -1899,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03902269899845123</v>
+        <v>0.03894839435815811</v>
       </c>
       <c r="C27" s="1">
         <v>36</v>
@@ -1925,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.03685477003455162</v>
+        <v>0.0367845930159092</v>
       </c>
       <c r="C28" s="1">
         <v>34</v>
@@ -1951,7 +1951,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03468684107065201</v>
+        <v>0.03462079539895058</v>
       </c>
       <c r="C29" s="1">
         <v>32</v>
@@ -1977,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03251891583204269</v>
+        <v>0.03245699405670166</v>
       </c>
       <c r="C30" s="1">
         <v>30</v>
@@ -2003,7 +2003,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03251891583204269</v>
+        <v>0.03245699405670166</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
@@ -2029,7 +2029,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.03035098686814308</v>
+        <v>0.03029319457709789</v>
       </c>
       <c r="C32" s="1">
         <v>28</v>
@@ -2055,7 +2055,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.03035098686814308</v>
+        <v>0.03029319457709789</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.03035098686814308</v>
+        <v>0.03029319457709789</v>
       </c>
       <c r="C34" s="1">
         <v>28</v>
@@ -2107,7 +2107,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.03035098686814308</v>
+        <v>0.03029319457709789</v>
       </c>
       <c r="C35" s="1">
         <v>28</v>
@@ -2133,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02818305976688862</v>
+        <v>0.02812939509749413</v>
       </c>
       <c r="C36" s="1">
         <v>26</v>
@@ -2159,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.01951134949922562</v>
+        <v>0.01947419717907906</v>
       </c>
       <c r="C37" s="1">
         <v>18</v>
@@ -2185,7 +2185,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01083963830024004</v>
+        <v>0.01081899832934141</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.008671710267663002</v>
+        <v>0.008655198849737644</v>
       </c>
       <c r="C39" s="1">
         <v>8</v>
@@ -2237,7 +2237,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>0.008671710267663002</v>
+        <v>0.008655198849737644</v>
       </c>
       <c r="C40" s="1">
         <v>8</v>
@@ -2263,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="2">
-        <v>0.004335855133831501</v>
+        <v>0.004327599424868822</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2289,7 +2289,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>0.004335855133831501</v>
+        <v>0.004327599424868822</v>
       </c>
       <c r="C42" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
fix cal temp error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -20,7 +20,7 @@
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-8eda70.o</t>
+    <t>lto-llvm-026b2c.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -261,7 +261,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-8eda70.o</c:v>
+                  <c:v>lto-llvm-026b2c.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -285,16 +285,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>84.00495910644531</c:v>
+                  <c:v>83.89513397216797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.87104797363281</c:v>
+                  <c:v>15.98002529144287</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.06199628114700317</c:v>
+                  <c:v>0.06242197379469872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06199628114700317</c:v>
+                  <c:v>0.06242197379469872</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -368,7 +368,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-8eda70.o</c:v>
+                  <c:v>lto-llvm-026b2c.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mc_w.l</c:v>
@@ -500,124 +500,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>89.52720642089844</c:v>
+                  <c:v>89.55635833740234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.877853393554688</c:v>
+                  <c:v>2.869843006134033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.442929744720459</c:v>
+                  <c:v>2.436129808425903</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.139997720718384</c:v>
+                  <c:v>2.13404107093811</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4370875358581543</c:v>
+                  <c:v>0.435870885848999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3613545298576355</c:v>
+                  <c:v>0.3603487014770508</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2466731518507004</c:v>
+                  <c:v>0.2459865361452103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2401817589998245</c:v>
+                  <c:v>0.2395132035017014</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.201233372092247</c:v>
+                  <c:v>0.2006732225418091</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1904143691062927</c:v>
+                  <c:v>0.1898843497037888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1341555714607239</c:v>
+                  <c:v>0.1337821483612061</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.119008980691433</c:v>
+                  <c:v>0.1186777129769325</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1081899851560593</c:v>
+                  <c:v>0.1078888326883316</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1060261800885201</c:v>
+                  <c:v>0.1057310551404953</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06707778573036194</c:v>
+                  <c:v>0.06689107418060303</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05409499257802963</c:v>
+                  <c:v>0.0539444163441658</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05409499257802963</c:v>
+                  <c:v>0.0539444163441658</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05193119123578072</c:v>
+                  <c:v>0.0517866387963295</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05193119123578072</c:v>
+                  <c:v>0.0517866387963295</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04760359227657318</c:v>
+                  <c:v>0.04747108742594719</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04327599331736565</c:v>
+                  <c:v>0.04315553233027458</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03894839435815811</c:v>
+                  <c:v>0.03883998095989227</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03894839435815811</c:v>
+                  <c:v>0.03883998095989227</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03894839435815811</c:v>
+                  <c:v>0.03883998095989227</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03894839435815811</c:v>
+                  <c:v>0.03883998095989227</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0367845930159092</c:v>
+                  <c:v>0.03668220341205597</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03462079539895058</c:v>
+                  <c:v>0.03452442586421967</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03245699405670166</c:v>
+                  <c:v>0.03236664831638336</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03245699405670166</c:v>
+                  <c:v>0.03236664831638336</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03029319457709789</c:v>
+                  <c:v>0.03020887263119221</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03029319457709789</c:v>
+                  <c:v>0.03020887263119221</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03029319457709789</c:v>
+                  <c:v>0.03020887263119221</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03029319457709789</c:v>
+                  <c:v>0.03020887263119221</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02812939509749413</c:v>
+                  <c:v>0.02805109694600105</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.01947419717907906</c:v>
+                  <c:v>0.01941999047994614</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01081899832934141</c:v>
+                  <c:v>0.01078888308256865</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.008655198849737644</c:v>
+                  <c:v>0.008631106466054916</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.008655198849737644</c:v>
+                  <c:v>0.008631106466054916</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.004327599424868822</c:v>
+                  <c:v>0.004315553233027458</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.004327599424868822</c:v>
+                  <c:v>0.004315553233027458</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -1087,25 +1087,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>84.00495910644531</v>
+        <v>83.89513397216797</v>
       </c>
       <c r="C3" s="1">
-        <v>5420</v>
+        <v>5376</v>
       </c>
       <c r="D3" s="1">
-        <v>82750</v>
+        <v>83008</v>
       </c>
       <c r="E3" s="1">
-        <v>82500</v>
+        <v>82746</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
       </c>
       <c r="G3" s="1">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="H3" s="1">
-        <v>5276</v>
+        <v>5220</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>15.87104797363281</v>
+        <v>15.98002529144287</v>
       </c>
       <c r="C4" s="1">
         <v>1024</v>
@@ -1139,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.06199628114700317</v>
+        <v>0.06242197379469872</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1165,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.06199628114700317</v>
+        <v>0.06242197379469872</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1275,25 +1275,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.52720642089844</v>
+        <v>89.55635833740234</v>
       </c>
       <c r="C3" s="1">
-        <v>82750</v>
+        <v>83008</v>
       </c>
       <c r="D3" s="1">
-        <v>5420</v>
+        <v>5376</v>
       </c>
       <c r="E3" s="1">
-        <v>82500</v>
+        <v>82746</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
       </c>
       <c r="G3" s="1">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="H3" s="1">
-        <v>5276</v>
+        <v>5220</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.877853393554688</v>
+        <v>2.869843006134033</v>
       </c>
       <c r="C4" s="1">
         <v>2660</v>
@@ -1327,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2.442929744720459</v>
+        <v>2.436129808425903</v>
       </c>
       <c r="C5" s="1">
         <v>2258</v>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2.139997720718384</v>
+        <v>2.13404107093811</v>
       </c>
       <c r="C6" s="1">
         <v>1978</v>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.4370875358581543</v>
+        <v>0.435870885848999</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3613545298576355</v>
+        <v>0.3603487014770508</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1431,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2466731518507004</v>
+        <v>0.2459865361452103</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1457,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2401817589998245</v>
+        <v>0.2395132035017014</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.201233372092247</v>
+        <v>0.2006732225418091</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1904143691062927</v>
+        <v>0.1898843497037888</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1341555714607239</v>
+        <v>0.1337821483612061</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.119008980691433</v>
+        <v>0.1186777129769325</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1081899851560593</v>
+        <v>0.1078888326883316</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1613,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1060261800885201</v>
+        <v>0.1057310551404953</v>
       </c>
       <c r="C16" s="1">
         <v>98</v>
@@ -1639,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.06707778573036194</v>
+        <v>0.06689107418060303</v>
       </c>
       <c r="C17" s="1">
         <v>62</v>
@@ -1665,7 +1665,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.05409499257802963</v>
+        <v>0.0539444163441658</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1691,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.05409499257802963</v>
+        <v>0.0539444163441658</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -1717,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.05193119123578072</v>
+        <v>0.0517866387963295</v>
       </c>
       <c r="C20" s="1">
         <v>48</v>
@@ -1743,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.05193119123578072</v>
+        <v>0.0517866387963295</v>
       </c>
       <c r="C21" s="1">
         <v>48</v>
@@ -1769,7 +1769,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04760359227657318</v>
+        <v>0.04747108742594719</v>
       </c>
       <c r="C22" s="1">
         <v>44</v>
@@ -1795,7 +1795,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04327599331736565</v>
+        <v>0.04315553233027458</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
@@ -1821,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.03894839435815811</v>
+        <v>0.03883998095989227</v>
       </c>
       <c r="C24" s="1">
         <v>36</v>
@@ -1847,7 +1847,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03894839435815811</v>
+        <v>0.03883998095989227</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1873,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03894839435815811</v>
+        <v>0.03883998095989227</v>
       </c>
       <c r="C26" s="1">
         <v>36</v>
@@ -1899,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03894839435815811</v>
+        <v>0.03883998095989227</v>
       </c>
       <c r="C27" s="1">
         <v>36</v>
@@ -1925,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.0367845930159092</v>
+        <v>0.03668220341205597</v>
       </c>
       <c r="C28" s="1">
         <v>34</v>
@@ -1951,7 +1951,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03462079539895058</v>
+        <v>0.03452442586421967</v>
       </c>
       <c r="C29" s="1">
         <v>32</v>
@@ -1977,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03245699405670166</v>
+        <v>0.03236664831638336</v>
       </c>
       <c r="C30" s="1">
         <v>30</v>
@@ -2003,7 +2003,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03245699405670166</v>
+        <v>0.03236664831638336</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
@@ -2029,7 +2029,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.03029319457709789</v>
+        <v>0.03020887263119221</v>
       </c>
       <c r="C32" s="1">
         <v>28</v>
@@ -2055,7 +2055,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.03029319457709789</v>
+        <v>0.03020887263119221</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.03029319457709789</v>
+        <v>0.03020887263119221</v>
       </c>
       <c r="C34" s="1">
         <v>28</v>
@@ -2107,7 +2107,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.03029319457709789</v>
+        <v>0.03020887263119221</v>
       </c>
       <c r="C35" s="1">
         <v>28</v>
@@ -2133,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02812939509749413</v>
+        <v>0.02805109694600105</v>
       </c>
       <c r="C36" s="1">
         <v>26</v>
@@ -2159,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.01947419717907906</v>
+        <v>0.01941999047994614</v>
       </c>
       <c r="C37" s="1">
         <v>18</v>
@@ -2185,7 +2185,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01081899832934141</v>
+        <v>0.01078888308256865</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.008655198849737644</v>
+        <v>0.008631106466054916</v>
       </c>
       <c r="C39" s="1">
         <v>8</v>
@@ -2237,7 +2237,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>0.008655198849737644</v>
+        <v>0.008631106466054916</v>
       </c>
       <c r="C40" s="1">
         <v>8</v>
@@ -2263,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="2">
-        <v>0.004327599424868822</v>
+        <v>0.004315553233027458</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2289,7 +2289,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>0.004327599424868822</v>
+        <v>0.004315553233027458</v>
       </c>
       <c r="C42" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
fix F temp cal error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -20,7 +20,7 @@
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-026b2c.o</t>
+    <t>lto-llvm-27d480.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -261,7 +261,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-026b2c.o</c:v>
+                  <c:v>lto-llvm-27d480.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -368,7 +368,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-026b2c.o</c:v>
+                  <c:v>lto-llvm-27d480.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mc_w.l</c:v>
@@ -500,124 +500,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>89.55635833740234</c:v>
+                  <c:v>89.55523681640625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.869843006134033</c:v>
+                  <c:v>2.870152473449707</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.436129808425903</c:v>
+                  <c:v>2.436392784118652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.13404107093811</c:v>
+                  <c:v>2.134271383285523</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.435870885848999</c:v>
+                  <c:v>0.4359179139137268</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3603487014770508</c:v>
+                  <c:v>0.3603875637054443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2459865361452103</c:v>
+                  <c:v>0.2460130751132965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2395132035017014</c:v>
+                  <c:v>0.2395390421152115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2006732225418091</c:v>
+                  <c:v>0.2006948739290237</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1898843497037888</c:v>
+                  <c:v>0.1899048388004303</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1337821483612061</c:v>
+                  <c:v>0.1337965875864029</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1186777129769325</c:v>
+                  <c:v>0.1186905205249786</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1078888326883316</c:v>
+                  <c:v>0.107900470495224</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1057310551404953</c:v>
+                  <c:v>0.1057424619793892</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06689107418060303</c:v>
+                  <c:v>0.06689829379320145</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0539444163441658</c:v>
+                  <c:v>0.053950235247612</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0539444163441658</c:v>
+                  <c:v>0.053950235247612</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0517866387963295</c:v>
+                  <c:v>0.05179222673177719</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0517866387963295</c:v>
+                  <c:v>0.05179222673177719</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04747108742594719</c:v>
+                  <c:v>0.04747620970010757</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04315553233027458</c:v>
+                  <c:v>0.04316018894314766</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03883998095989227</c:v>
+                  <c:v>0.03884417191147804</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03883998095989227</c:v>
+                  <c:v>0.03884417191147804</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03883998095989227</c:v>
+                  <c:v>0.03884417191147804</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03883998095989227</c:v>
+                  <c:v>0.03884417191147804</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03668220341205597</c:v>
+                  <c:v>0.03668615967035294</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03452442586421967</c:v>
+                  <c:v>0.03452815115451813</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03236664831638336</c:v>
+                  <c:v>0.03237014263868332</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03236664831638336</c:v>
+                  <c:v>0.03237014263868332</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03020887263119221</c:v>
+                  <c:v>0.03021213226020336</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03020887263119221</c:v>
+                  <c:v>0.03021213226020336</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03020887263119221</c:v>
+                  <c:v>0.03021213226020336</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03020887263119221</c:v>
+                  <c:v>0.03021213226020336</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02805109694600105</c:v>
+                  <c:v>0.02805412374436855</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.01941999047994614</c:v>
+                  <c:v>0.01942208595573902</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01078888308256865</c:v>
+                  <c:v>0.01079004723578692</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.008631106466054916</c:v>
+                  <c:v>0.008632037788629532</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.008631106466054916</c:v>
+                  <c:v>0.008632037788629532</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.004315553233027458</c:v>
+                  <c:v>0.004316018894314766</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.004315553233027458</c:v>
+                  <c:v>0.004316018894314766</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -1093,10 +1093,10 @@
         <v>5376</v>
       </c>
       <c r="D3" s="1">
-        <v>83008</v>
+        <v>82998</v>
       </c>
       <c r="E3" s="1">
-        <v>82746</v>
+        <v>82736</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1275,16 +1275,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.55635833740234</v>
+        <v>89.55523681640625</v>
       </c>
       <c r="C3" s="1">
-        <v>83008</v>
+        <v>82998</v>
       </c>
       <c r="D3" s="1">
         <v>5376</v>
       </c>
       <c r="E3" s="1">
-        <v>82746</v>
+        <v>82736</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.869843006134033</v>
+        <v>2.870152473449707</v>
       </c>
       <c r="C4" s="1">
         <v>2660</v>
@@ -1327,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2.436129808425903</v>
+        <v>2.436392784118652</v>
       </c>
       <c r="C5" s="1">
         <v>2258</v>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2.13404107093811</v>
+        <v>2.134271383285523</v>
       </c>
       <c r="C6" s="1">
         <v>1978</v>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.435870885848999</v>
+        <v>0.4359179139137268</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3603487014770508</v>
+        <v>0.3603875637054443</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1431,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2459865361452103</v>
+        <v>0.2460130751132965</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1457,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2395132035017014</v>
+        <v>0.2395390421152115</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.2006732225418091</v>
+        <v>0.2006948739290237</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1898843497037888</v>
+        <v>0.1899048388004303</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1337821483612061</v>
+        <v>0.1337965875864029</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1186777129769325</v>
+        <v>0.1186905205249786</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.1078888326883316</v>
+        <v>0.107900470495224</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1613,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1057310551404953</v>
+        <v>0.1057424619793892</v>
       </c>
       <c r="C16" s="1">
         <v>98</v>
@@ -1639,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.06689107418060303</v>
+        <v>0.06689829379320145</v>
       </c>
       <c r="C17" s="1">
         <v>62</v>
@@ -1665,7 +1665,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.0539444163441658</v>
+        <v>0.053950235247612</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1691,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.0539444163441658</v>
+        <v>0.053950235247612</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -1717,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.0517866387963295</v>
+        <v>0.05179222673177719</v>
       </c>
       <c r="C20" s="1">
         <v>48</v>
@@ -1743,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.0517866387963295</v>
+        <v>0.05179222673177719</v>
       </c>
       <c r="C21" s="1">
         <v>48</v>
@@ -1769,7 +1769,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04747108742594719</v>
+        <v>0.04747620970010757</v>
       </c>
       <c r="C22" s="1">
         <v>44</v>
@@ -1795,7 +1795,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04315553233027458</v>
+        <v>0.04316018894314766</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
@@ -1821,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.03883998095989227</v>
+        <v>0.03884417191147804</v>
       </c>
       <c r="C24" s="1">
         <v>36</v>
@@ -1847,7 +1847,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03883998095989227</v>
+        <v>0.03884417191147804</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1873,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03883998095989227</v>
+        <v>0.03884417191147804</v>
       </c>
       <c r="C26" s="1">
         <v>36</v>
@@ -1899,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03883998095989227</v>
+        <v>0.03884417191147804</v>
       </c>
       <c r="C27" s="1">
         <v>36</v>
@@ -1925,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.03668220341205597</v>
+        <v>0.03668615967035294</v>
       </c>
       <c r="C28" s="1">
         <v>34</v>
@@ -1951,7 +1951,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03452442586421967</v>
+        <v>0.03452815115451813</v>
       </c>
       <c r="C29" s="1">
         <v>32</v>
@@ -1977,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03236664831638336</v>
+        <v>0.03237014263868332</v>
       </c>
       <c r="C30" s="1">
         <v>30</v>
@@ -2003,7 +2003,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03236664831638336</v>
+        <v>0.03237014263868332</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
@@ -2029,7 +2029,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.03020887263119221</v>
+        <v>0.03021213226020336</v>
       </c>
       <c r="C32" s="1">
         <v>28</v>
@@ -2055,7 +2055,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.03020887263119221</v>
+        <v>0.03021213226020336</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.03020887263119221</v>
+        <v>0.03021213226020336</v>
       </c>
       <c r="C34" s="1">
         <v>28</v>
@@ -2107,7 +2107,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.03020887263119221</v>
+        <v>0.03021213226020336</v>
       </c>
       <c r="C35" s="1">
         <v>28</v>
@@ -2133,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02805109694600105</v>
+        <v>0.02805412374436855</v>
       </c>
       <c r="C36" s="1">
         <v>26</v>
@@ -2159,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.01941999047994614</v>
+        <v>0.01942208595573902</v>
       </c>
       <c r="C37" s="1">
         <v>18</v>
@@ -2185,7 +2185,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01078888308256865</v>
+        <v>0.01079004723578692</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.008631106466054916</v>
+        <v>0.008632037788629532</v>
       </c>
       <c r="C39" s="1">
         <v>8</v>
@@ -2237,7 +2237,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>0.008631106466054916</v>
+        <v>0.008632037788629532</v>
       </c>
       <c r="C40" s="1">
         <v>8</v>
@@ -2263,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="2">
-        <v>0.004315553233027458</v>
+        <v>0.004316018894314766</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2289,7 +2289,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>0.004315553233027458</v>
+        <v>0.004316018894314766</v>
       </c>
       <c r="C42" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
fix quick work temp and time flash error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -20,7 +20,7 @@
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-27d480.o</t>
+    <t>lto-llvm-736de3.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -261,7 +261,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-27d480.o</c:v>
+                  <c:v>lto-llvm-736de3.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -285,16 +285,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>83.89513397216797</c:v>
+                  <c:v>83.90517425537109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.98002529144287</c:v>
+                  <c:v>15.97005653381348</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.06242197379469872</c:v>
+                  <c:v>0.06238303333520889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06242197379469872</c:v>
+                  <c:v>0.06238303333520889</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -368,7 +368,7 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-27d480.o</c:v>
+                  <c:v>lto-llvm-736de3.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mc_w.l</c:v>
@@ -500,124 +500,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>89.55523681640625</c:v>
+                  <c:v>89.59117126464844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.870152473449707</c:v>
+                  <c:v>2.860276460647583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.436392784118652</c:v>
+                  <c:v>2.428009271621704</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.134271383285523</c:v>
+                  <c:v>2.126927375793457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4359179139137268</c:v>
+                  <c:v>0.4344179332256317</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3603875637054443</c:v>
+                  <c:v>0.3591475188732147</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2460130751132965</c:v>
+                  <c:v>0.2451665699481964</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2395390421152115</c:v>
+                  <c:v>0.2387148141860962</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2006948739290237</c:v>
+                  <c:v>0.2000042945146561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1899048388004303</c:v>
+                  <c:v>0.1892513781785965</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1337965875864029</c:v>
+                  <c:v>0.1333362013101578</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1186905205249786</c:v>
+                  <c:v>0.1182821169495583</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.107900470495224</c:v>
+                  <c:v>0.1075291931629181</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1057424619793892</c:v>
+                  <c:v>0.1053786128759384</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06689829379320145</c:v>
+                  <c:v>0.06666810065507889</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.053950235247612</c:v>
+                  <c:v>0.05376459658145905</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.053950235247612</c:v>
+                  <c:v>0.05376459658145905</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05179222673177719</c:v>
+                  <c:v>0.05161401256918907</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05179222673177719</c:v>
+                  <c:v>0.05161401256918907</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04747620970010757</c:v>
+                  <c:v>0.04731284454464912</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04316018894314766</c:v>
+                  <c:v>0.04301167652010918</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03884417191147804</c:v>
+                  <c:v>0.03871050849556923</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03884417191147804</c:v>
+                  <c:v>0.03871050849556923</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03884417191147804</c:v>
+                  <c:v>0.03871050849556923</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03884417191147804</c:v>
+                  <c:v>0.03871050849556923</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03668615967035294</c:v>
+                  <c:v>0.03655992448329926</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03452815115451813</c:v>
+                  <c:v>0.03440934047102928</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03237014263868332</c:v>
+                  <c:v>0.03225875645875931</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03237014263868332</c:v>
+                  <c:v>0.03225875645875931</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03021213226020336</c:v>
+                  <c:v>0.03010817430913448</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03021213226020336</c:v>
+                  <c:v>0.03010817430913448</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.03021213226020336</c:v>
+                  <c:v>0.03010817430913448</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.03021213226020336</c:v>
+                  <c:v>0.03010817430913448</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02805412374436855</c:v>
+                  <c:v>0.02795759029686451</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.01942208595573902</c:v>
+                  <c:v>0.01935525424778462</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01079004723578692</c:v>
+                  <c:v>0.01075291913002729</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.008632037788629532</c:v>
+                  <c:v>0.00860233511775732</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.008632037788629532</c:v>
+                  <c:v>0.00860233511775732</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.004316018894314766</c:v>
+                  <c:v>0.00430116755887866</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.004316018894314766</c:v>
+                  <c:v>0.00430116755887866</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -1087,16 +1087,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>83.89513397216797</v>
+        <v>83.90517425537109</v>
       </c>
       <c r="C3" s="1">
-        <v>5376</v>
+        <v>5380</v>
       </c>
       <c r="D3" s="1">
-        <v>82998</v>
+        <v>83318</v>
       </c>
       <c r="E3" s="1">
-        <v>82736</v>
+        <v>83056</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1105,7 +1105,7 @@
         <v>156</v>
       </c>
       <c r="H3" s="1">
-        <v>5220</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1113,7 +1113,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>15.98002529144287</v>
+        <v>15.97005653381348</v>
       </c>
       <c r="C4" s="1">
         <v>1024</v>
@@ -1139,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.06242197379469872</v>
+        <v>0.06238303333520889</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1165,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.06242197379469872</v>
+        <v>0.06238303333520889</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1275,16 +1275,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>89.55523681640625</v>
+        <v>89.59117126464844</v>
       </c>
       <c r="C3" s="1">
-        <v>82998</v>
+        <v>83318</v>
       </c>
       <c r="D3" s="1">
-        <v>5376</v>
+        <v>5380</v>
       </c>
       <c r="E3" s="1">
-        <v>82736</v>
+        <v>83056</v>
       </c>
       <c r="F3" s="1">
         <v>106</v>
@@ -1293,7 +1293,7 @@
         <v>156</v>
       </c>
       <c r="H3" s="1">
-        <v>5220</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.870152473449707</v>
+        <v>2.860276460647583</v>
       </c>
       <c r="C4" s="1">
         <v>2660</v>
@@ -1327,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2.436392784118652</v>
+        <v>2.428009271621704</v>
       </c>
       <c r="C5" s="1">
         <v>2258</v>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2.134271383285523</v>
+        <v>2.126927375793457</v>
       </c>
       <c r="C6" s="1">
         <v>1978</v>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.4359179139137268</v>
+        <v>0.4344179332256317</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3603875637054443</v>
+        <v>0.3591475188732147</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1431,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2460130751132965</v>
+        <v>0.2451665699481964</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1457,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2395390421152115</v>
+        <v>0.2387148141860962</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.2006948739290237</v>
+        <v>0.2000042945146561</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1899048388004303</v>
+        <v>0.1892513781785965</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1337965875864029</v>
+        <v>0.1333362013101578</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1186905205249786</v>
+        <v>0.1182821169495583</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1587,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.107900470495224</v>
+        <v>0.1075291931629181</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1613,7 +1613,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1057424619793892</v>
+        <v>0.1053786128759384</v>
       </c>
       <c r="C16" s="1">
         <v>98</v>
@@ -1639,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.06689829379320145</v>
+        <v>0.06666810065507889</v>
       </c>
       <c r="C17" s="1">
         <v>62</v>
@@ -1665,7 +1665,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.053950235247612</v>
+        <v>0.05376459658145905</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1691,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.053950235247612</v>
+        <v>0.05376459658145905</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -1717,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.05179222673177719</v>
+        <v>0.05161401256918907</v>
       </c>
       <c r="C20" s="1">
         <v>48</v>
@@ -1743,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.05179222673177719</v>
+        <v>0.05161401256918907</v>
       </c>
       <c r="C21" s="1">
         <v>48</v>
@@ -1769,7 +1769,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04747620970010757</v>
+        <v>0.04731284454464912</v>
       </c>
       <c r="C22" s="1">
         <v>44</v>
@@ -1795,7 +1795,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04316018894314766</v>
+        <v>0.04301167652010918</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
@@ -1821,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.03884417191147804</v>
+        <v>0.03871050849556923</v>
       </c>
       <c r="C24" s="1">
         <v>36</v>
@@ -1847,7 +1847,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03884417191147804</v>
+        <v>0.03871050849556923</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1873,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03884417191147804</v>
+        <v>0.03871050849556923</v>
       </c>
       <c r="C26" s="1">
         <v>36</v>
@@ -1899,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03884417191147804</v>
+        <v>0.03871050849556923</v>
       </c>
       <c r="C27" s="1">
         <v>36</v>
@@ -1925,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.03668615967035294</v>
+        <v>0.03655992448329926</v>
       </c>
       <c r="C28" s="1">
         <v>34</v>
@@ -1951,7 +1951,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03452815115451813</v>
+        <v>0.03440934047102928</v>
       </c>
       <c r="C29" s="1">
         <v>32</v>
@@ -1977,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03237014263868332</v>
+        <v>0.03225875645875931</v>
       </c>
       <c r="C30" s="1">
         <v>30</v>
@@ -2003,7 +2003,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03237014263868332</v>
+        <v>0.03225875645875931</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
@@ -2029,7 +2029,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.03021213226020336</v>
+        <v>0.03010817430913448</v>
       </c>
       <c r="C32" s="1">
         <v>28</v>
@@ -2055,7 +2055,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.03021213226020336</v>
+        <v>0.03010817430913448</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.03021213226020336</v>
+        <v>0.03010817430913448</v>
       </c>
       <c r="C34" s="1">
         <v>28</v>
@@ -2107,7 +2107,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.03021213226020336</v>
+        <v>0.03010817430913448</v>
       </c>
       <c r="C35" s="1">
         <v>28</v>
@@ -2133,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02805412374436855</v>
+        <v>0.02795759029686451</v>
       </c>
       <c r="C36" s="1">
         <v>26</v>
@@ -2159,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.01942208595573902</v>
+        <v>0.01935525424778462</v>
       </c>
       <c r="C37" s="1">
         <v>18</v>
@@ -2185,7 +2185,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01079004723578692</v>
+        <v>0.01075291913002729</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
@@ -2211,7 +2211,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>0.008632037788629532</v>
+        <v>0.00860233511775732</v>
       </c>
       <c r="C39" s="1">
         <v>8</v>
@@ -2237,7 +2237,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>0.008632037788629532</v>
+        <v>0.00860233511775732</v>
       </c>
       <c r="C40" s="1">
         <v>8</v>
@@ -2263,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="2">
-        <v>0.004316018894314766</v>
+        <v>0.00430116755887866</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2289,7 +2289,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>0.004316018894314766</v>
+        <v>0.00430116755887866</v>
       </c>
       <c r="C42" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
change bootloader,add pc/usrt4/usrt5 function
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-28d337.o</t>
+    <t>lto-llvm-715488.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -32,12 +32,12 @@
     <t>stdout.o</t>
   </si>
   <si>
-    <t>printfa.o</t>
-  </si>
-  <si>
     <t>mf_w.l</t>
   </si>
   <si>
+    <t>printf6.o</t>
+  </si>
+  <si>
     <t>dadd.o</t>
   </si>
   <si>
@@ -62,9 +62,6 @@
     <t>fmul.o</t>
   </si>
   <si>
-    <t>uldiv.o</t>
-  </si>
-  <si>
     <t>dfixi.o</t>
   </si>
   <si>
@@ -74,19 +71,13 @@
     <t>dfixui.o</t>
   </si>
   <si>
-    <t>dfixul.o</t>
-  </si>
-  <si>
-    <t>cdrcmple.o</t>
-  </si>
-  <si>
     <t>uidiv.o</t>
   </si>
   <si>
     <t>ffixui.o</t>
   </si>
   <si>
-    <t>f2d.o</t>
+    <t>puts.o</t>
   </si>
   <si>
     <t>memseta.o</t>
@@ -260,11 +251,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$44</c:f>
+              <c:f>ram_percent!$A$3:$A$41</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-28d337.o</c:v>
+                  <c:v>lto-llvm-715488.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -275,7 +266,7 @@
                 <c:pt idx="3">
                   <c:v>stdout.o</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="38">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -283,23 +274,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$44</c:f>
+              <c:f>ram_percent!$B$3:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>84.13284301757813</c:v>
+                  <c:v>92.76246643066406</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.7441577911377</c:v>
+                  <c:v>7.181429386138916</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.06150061637163162</c:v>
+                  <c:v>0.02805245853960514</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06150061637163162</c:v>
-                </c:pt>
-                <c:pt idx="41">
+                  <c:v>0.02805245853960514</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -367,20 +358,20 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$44</c:f>
+              <c:f>flash_percent!$A$3:$A$41</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-28d337.o</c:v>
+                  <c:v>lto-llvm-715488.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>mf_w.l</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>mc_w.l</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>printfa.o</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>mf_w.l</c:v>
+                  <c:v>printf6.o</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>startup_at32f415.o</c:v>
@@ -410,90 +401,81 @@
                   <c:v>fmul.o</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>uldiv.o</c:v>
+                  <c:v>dfixi.o</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>dfixi.o</c:v>
+                  <c:v>ffixi.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>ffixi.o</c:v>
+                  <c:v>dfixui.o</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>dfixui.o</c:v>
+                  <c:v>uidiv.o</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>dfixul.o</c:v>
+                  <c:v>ffixui.o</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>cdrcmple.o</c:v>
+                  <c:v>puts.o</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>uidiv.o</c:v>
+                  <c:v>memseta.o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>ffixui.o</c:v>
+                  <c:v>memcpya.o</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>f2d.o</c:v>
+                  <c:v>llsshr.o</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>memseta.o</c:v>
+                  <c:v>init.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>memcpya.o</c:v>
+                  <c:v>dflti.o</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>llsshr.o</c:v>
+                  <c:v>llushr.o</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>init.o</c:v>
+                  <c:v>llshl.o</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>dflti.o</c:v>
+                  <c:v>handlers.o</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>llushr.o</c:v>
+                  <c:v>fcmplt.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>llshl.o</c:v>
+                  <c:v>fcmple.o</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>handlers.o</c:v>
+                  <c:v>fcmpgt.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>fcmplt.o</c:v>
+                  <c:v>fcmpge.o</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>fcmple.o</c:v>
+                  <c:v>dfltui.o</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>fcmpgt.o</c:v>
+                  <c:v>fflti.o</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>fcmpge.o</c:v>
+                  <c:v>ffltui.o</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>dfltui.o</c:v>
+                  <c:v>entry9a.o</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>fflti.o</c:v>
+                  <c:v>entry2.o</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>ffltui.o</c:v>
+                  <c:v>stdout.o</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>entry9a.o</c:v>
+                  <c:v>entry5.o</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>entry2.o</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>stdout.o</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>entry5.o</c:v>
-                </c:pt>
-                <c:pt idx="41">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -501,134 +483,125 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$44</c:f>
+              <c:f>flash_percent!$B$3:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>90.36739349365234</c:v>
+                  <c:v>85.02059936523438</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.626356363296509</c:v>
+                  <c:v>4.284380912780762</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.229440927505493</c:v>
+                  <c:v>2.745464086532593</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.990501642227173</c:v>
+                  <c:v>1.971452593803406</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3988902270793915</c:v>
+                  <c:v>0.919707715511322</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3297755718231201</c:v>
+                  <c:v>0.760352373123169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2251162678003311</c:v>
+                  <c:v>0.51904296875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2191921472549439</c:v>
+                  <c:v>0.5053839087486267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1836474686861038</c:v>
+                  <c:v>0.4234297871589661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1737739592790604</c:v>
+                  <c:v>0.400664746761322</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1224316507577896</c:v>
+                  <c:v>0.282286524772644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1086087226867676</c:v>
+                  <c:v>0.2504154741764069</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.09873519837856293</c:v>
+                  <c:v>0.2276504188776016</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.09676049649715424</c:v>
+                  <c:v>0.141143262386322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06121582537889481</c:v>
+                  <c:v>0.1138252094388008</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04936759918928146</c:v>
+                  <c:v>0.1138252094388008</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.04936759918928146</c:v>
+                  <c:v>0.1001661866903305</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.04739289730787277</c:v>
+                  <c:v>0.09106016904115677</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.04739289730787277</c:v>
+                  <c:v>0.08195415139198303</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04344348981976509</c:v>
+                  <c:v>0.08195415139198303</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.03949408233165741</c:v>
+                  <c:v>0.08195415139198303</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.03751937672495842</c:v>
+                  <c:v>0.08195415139198303</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.03554467111825943</c:v>
+                  <c:v>0.08195415139198303</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03554467111825943</c:v>
+                  <c:v>0.07740114629268646</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03554467111825943</c:v>
+                  <c:v>0.0728481337428093</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03554467111825943</c:v>
+                  <c:v>0.06829512864351273</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03356996923685074</c:v>
+                  <c:v>0.06829512864351273</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03159526363015175</c:v>
+                  <c:v>0.06374211609363556</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.02962055988609791</c:v>
+                  <c:v>0.06374211609363556</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.02962055988609791</c:v>
+                  <c:v>0.06374211609363556</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.02764585614204407</c:v>
+                  <c:v>0.06374211609363556</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.02764585614204407</c:v>
+                  <c:v>0.05918911099433899</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.02764585614204407</c:v>
+                  <c:v>0.04097707569599152</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02764585614204407</c:v>
+                  <c:v>0.02276504226028919</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.02567115239799023</c:v>
+                  <c:v>0.01821203343570232</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01777233555912972</c:v>
+                  <c:v>0.01821203343570232</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.009873520582914352</c:v>
+                  <c:v>0.009106016717851162</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.007898815907537937</c:v>
+                  <c:v>0.009106016717851162</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.007898815907537937</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.003949407953768969</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.003949407953768969</c:v>
-                </c:pt>
-                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -733,8 +706,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H44" totalsRowCount="1">
-  <autoFilter ref="A2:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H41" totalsRowCount="1">
+  <autoFilter ref="A2:H40"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -750,8 +723,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H44" totalsRowCount="1">
-  <autoFilter ref="A2:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H41" totalsRowCount="1">
+  <autoFilter ref="A2:H40"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1051,7 +1024,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1067,28 +1040,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1096,25 +1069,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>84.13284301757813</v>
+        <v>92.76246643066406</v>
       </c>
       <c r="C3" s="1">
-        <v>5472</v>
+        <v>13227</v>
       </c>
       <c r="D3" s="1">
-        <v>91525</v>
+        <v>37347</v>
       </c>
       <c r="E3" s="1">
-        <v>91200</v>
+        <v>37064</v>
       </c>
       <c r="F3" s="1">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="H3" s="1">
-        <v>5316</v>
+        <v>13092</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1122,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>15.7441577911377</v>
+        <v>7.181429386138916</v>
       </c>
       <c r="C4" s="1">
         <v>1024</v>
@@ -1148,16 +1121,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.06150061637163162</v>
+        <v>0.02805245853960514</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>2660</v>
+        <v>1206</v>
       </c>
       <c r="E5" s="1">
-        <v>2656</v>
+        <v>1202</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1174,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.06150061637163162</v>
+        <v>0.02805245853960514</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1195,35 +1168,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C44">
+      <c r="C41">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D44">
+      <c r="D41">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E44">
+      <c r="E41">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F41">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G44">
+      <c r="G41">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H44">
+      <c r="H41">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1239,7 +1212,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1255,28 +1228,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1284,48 +1257,48 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>90.36739349365234</v>
+        <v>85.02059936523438</v>
       </c>
       <c r="C3" s="1">
-        <v>91525</v>
+        <v>37347</v>
       </c>
       <c r="D3" s="1">
-        <v>5472</v>
+        <v>13227</v>
       </c>
       <c r="E3" s="1">
-        <v>91200</v>
+        <v>37064</v>
       </c>
       <c r="F3" s="1">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="H3" s="1">
-        <v>5316</v>
+        <v>13092</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>2.626356363296509</v>
+        <v>4.284380912780762</v>
       </c>
       <c r="C4" s="1">
-        <v>2660</v>
+        <v>1882</v>
       </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>2656</v>
+        <v>1882</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -1333,25 +1306,25 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>2.229440927505493</v>
+        <v>2.745464086532593</v>
       </c>
       <c r="C5" s="1">
-        <v>2258</v>
+        <v>1206</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>2258</v>
+        <v>1202</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1362,16 +1335,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>1.990501642227173</v>
+        <v>1.971452593803406</v>
       </c>
       <c r="C6" s="1">
-        <v>2016</v>
+        <v>866</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>2016</v>
+        <v>866</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1388,7 +1361,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.3988902270793915</v>
+        <v>0.919707715511322</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
@@ -1414,7 +1387,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3297755718231201</v>
+        <v>0.760352373123169</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1440,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.2251162678003311</v>
+        <v>0.51904296875</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1466,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2191921472549439</v>
+        <v>0.5053839087486267</v>
       </c>
       <c r="C10" s="1">
         <v>222</v>
@@ -1492,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.1836474686861038</v>
+        <v>0.4234297871589661</v>
       </c>
       <c r="C11" s="1">
         <v>186</v>
@@ -1518,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1737739592790604</v>
+        <v>0.400664746761322</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -1544,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1224316507577896</v>
+        <v>0.282286524772644</v>
       </c>
       <c r="C13" s="1">
         <v>124</v>
@@ -1570,7 +1543,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.1086087226867676</v>
+        <v>0.2504154741764069</v>
       </c>
       <c r="C14" s="1">
         <v>110</v>
@@ -1596,7 +1569,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.09873519837856293</v>
+        <v>0.2276504188776016</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1622,16 +1595,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.09676049649715424</v>
+        <v>0.141143262386322</v>
       </c>
       <c r="C16" s="1">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1648,16 +1621,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.06121582537889481</v>
+        <v>0.1138252094388008</v>
       </c>
       <c r="C17" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1674,7 +1647,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.04936759918928146</v>
+        <v>0.1138252094388008</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
@@ -1700,16 +1673,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.04936759918928146</v>
+        <v>0.1001661866903305</v>
       </c>
       <c r="C19" s="1">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1726,16 +1699,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.04739289730787277</v>
+        <v>0.09106016904115677</v>
       </c>
       <c r="C20" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1752,16 +1725,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.04739289730787277</v>
+        <v>0.08195415139198303</v>
       </c>
       <c r="C21" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1778,16 +1751,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.04344348981976509</v>
+        <v>0.08195415139198303</v>
       </c>
       <c r="C22" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1804,16 +1777,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.03949408233165741</v>
+        <v>0.08195415139198303</v>
       </c>
       <c r="C23" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1830,16 +1803,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.03751937672495842</v>
+        <v>0.08195415139198303</v>
       </c>
       <c r="C24" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1856,7 +1829,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.03554467111825943</v>
+        <v>0.08195415139198303</v>
       </c>
       <c r="C25" s="1">
         <v>36</v>
@@ -1882,16 +1855,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.03554467111825943</v>
+        <v>0.07740114629268646</v>
       </c>
       <c r="C26" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1908,16 +1881,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.03554467111825943</v>
+        <v>0.0728481337428093</v>
       </c>
       <c r="C27" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1934,16 +1907,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.03554467111825943</v>
+        <v>0.06829512864351273</v>
       </c>
       <c r="C28" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1960,16 +1933,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.03356996923685074</v>
+        <v>0.06829512864351273</v>
       </c>
       <c r="C29" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1986,16 +1959,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.03159526363015175</v>
+        <v>0.06374211609363556</v>
       </c>
       <c r="C30" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2012,16 +1985,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.02962055988609791</v>
+        <v>0.06374211609363556</v>
       </c>
       <c r="C31" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2038,16 +2011,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.02962055988609791</v>
+        <v>0.06374211609363556</v>
       </c>
       <c r="C32" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2064,7 +2037,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.02764585614204407</v>
+        <v>0.06374211609363556</v>
       </c>
       <c r="C33" s="1">
         <v>28</v>
@@ -2090,16 +2063,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.02764585614204407</v>
+        <v>0.05918911099433899</v>
       </c>
       <c r="C34" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2116,16 +2089,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.02764585614204407</v>
+        <v>0.04097707569599152</v>
       </c>
       <c r="C35" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2142,16 +2115,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02764585614204407</v>
+        <v>0.02276504226028919</v>
       </c>
       <c r="C36" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2168,16 +2141,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>0.02567115239799023</v>
+        <v>0.01821203343570232</v>
       </c>
       <c r="C37" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2194,16 +2167,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01777233555912972</v>
+        <v>0.01821203343570232</v>
       </c>
       <c r="C38" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2217,25 +2190,25 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B39" s="2">
-        <v>0.009873520582914352</v>
+        <v>0.009106016717851162</v>
       </c>
       <c r="C39" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E39" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
       </c>
       <c r="G39" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
@@ -2243,19 +2216,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2">
-        <v>0.007898815907537937</v>
+        <v>0.009106016717851162</v>
       </c>
       <c r="C40" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -2268,112 +2241,34 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
-        <v>0.007898815907537937</v>
-      </c>
-      <c r="C41" s="1">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <v>8</v>
-      </c>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0.003949407953768969</v>
-      </c>
-      <c r="C42" s="1">
-        <v>4</v>
-      </c>
-      <c r="D42" s="1">
-        <v>4</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1">
-        <v>4</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2">
-        <v>0.003949407953768969</v>
-      </c>
-      <c r="C43" s="1">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <v>4</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
+      <c r="B41">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C44">
+      <c r="C41">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D44">
+      <c r="D41">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E44">
+      <c r="E41">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F41">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G44">
+      <c r="G41">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H44">
+      <c r="H41">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
change pid range,add sleep function ,fix cal error,change flash time
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-715488.o</t>
+    <t>lto-llvm-132006.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
@@ -44,18 +44,12 @@
     <t>dmul.o</t>
   </si>
   <si>
-    <t>ddiv.o</t>
-  </si>
-  <si>
     <t>depilogue.o</t>
   </si>
   <si>
     <t>fadd.o</t>
   </si>
   <si>
-    <t>fdiv.o</t>
-  </si>
-  <si>
     <t>fepilogue.o</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
   </si>
   <si>
     <t>dfixi.o</t>
-  </si>
-  <si>
-    <t>ffixi.o</t>
   </si>
   <si>
     <t>dfixui.o</t>
@@ -251,11 +242,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$41</c:f>
+              <c:f>ram_percent!$A$3:$A$38</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-715488.o</c:v>
+                  <c:v>lto-llvm-132006.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
@@ -266,7 +257,7 @@
                 <c:pt idx="3">
                   <c:v>stdout.o</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="35">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -274,23 +265,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$41</c:f>
+              <c:f>ram_percent!$B$3:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>92.76246643066406</c:v>
+                  <c:v>86.59014129638672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.181429386138916</c:v>
+                  <c:v>13.3576831817627</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02805245853960514</c:v>
+                  <c:v>0.02608922496438026</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02805245853960514</c:v>
-                </c:pt>
-                <c:pt idx="38">
+                  <c:v>0.02608922496438026</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -358,11 +349,11 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$41</c:f>
+              <c:f>flash_percent!$A$3:$A$38</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-715488.o</c:v>
+                  <c:v>lto-llvm-132006.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mf_w.l</c:v>
@@ -383,99 +374,90 @@
                   <c:v>dmul.o</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>ddiv.o</c:v>
+                  <c:v>depilogue.o</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>depilogue.o</c:v>
+                  <c:v>fadd.o</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>fadd.o</c:v>
+                  <c:v>fepilogue.o</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>fdiv.o</c:v>
+                  <c:v>fmul.o</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>fepilogue.o</c:v>
+                  <c:v>dfixi.o</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>fmul.o</c:v>
+                  <c:v>dfixui.o</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>dfixi.o</c:v>
+                  <c:v>uidiv.o</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>ffixi.o</c:v>
+                  <c:v>ffixui.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>dfixui.o</c:v>
+                  <c:v>puts.o</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>uidiv.o</c:v>
+                  <c:v>memseta.o</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>ffixui.o</c:v>
+                  <c:v>memcpya.o</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>puts.o</c:v>
+                  <c:v>llsshr.o</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>memseta.o</c:v>
+                  <c:v>init.o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>memcpya.o</c:v>
+                  <c:v>dflti.o</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>llsshr.o</c:v>
+                  <c:v>llushr.o</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>init.o</c:v>
+                  <c:v>llshl.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>dflti.o</c:v>
+                  <c:v>handlers.o</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>llushr.o</c:v>
+                  <c:v>fcmplt.o</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>llshl.o</c:v>
+                  <c:v>fcmple.o</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>handlers.o</c:v>
+                  <c:v>fcmpgt.o</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>fcmplt.o</c:v>
+                  <c:v>fcmpge.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>fcmple.o</c:v>
+                  <c:v>dfltui.o</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>fcmpgt.o</c:v>
+                  <c:v>fflti.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>fcmpge.o</c:v>
+                  <c:v>ffltui.o</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>dfltui.o</c:v>
+                  <c:v>entry9a.o</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>fflti.o</c:v>
+                  <c:v>entry2.o</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>ffltui.o</c:v>
+                  <c:v>stdout.o</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>entry9a.o</c:v>
+                  <c:v>entry5.o</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>entry2.o</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>stdout.o</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>entry5.o</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -483,125 +465,116 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$41</c:f>
+              <c:f>flash_percent!$B$3:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>85.02059936523438</c:v>
+                  <c:v>91.644287109375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.284380912780762</c:v>
+                  <c:v>2.145228862762451</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.745464086532593</c:v>
+                  <c:v>1.741013407707214</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.971452593803406</c:v>
+                  <c:v>1.25018048286438</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.919707715511322</c:v>
+                  <c:v>0.5832250714302063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.760352373123169</c:v>
+                  <c:v>0.4821712076663971</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51904296875</c:v>
+                  <c:v>0.3291468024253845</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5053839087486267</c:v>
+                  <c:v>0.2685145139694214</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4234297871589661</c:v>
+                  <c:v>0.2540782392024994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.400664746761322</c:v>
+                  <c:v>0.1587989032268524</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.282286524772644</c:v>
+                  <c:v>0.1443626433610916</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2504154741764069</c:v>
+                  <c:v>0.08950483798980713</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2276504188776016</c:v>
+                  <c:v>0.07218132168054581</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.141143262386322</c:v>
+                  <c:v>0.06351955980062485</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1138252094388008</c:v>
+                  <c:v>0.05774505436420441</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1138252094388008</c:v>
+                  <c:v>0.05197054892778397</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1001661866903305</c:v>
+                  <c:v>0.05197054892778397</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.09106016904115677</c:v>
+                  <c:v>0.05197054892778397</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.08195415139198303</c:v>
+                  <c:v>0.05197054892778397</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08195415139198303</c:v>
+                  <c:v>0.05197054892778397</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.08195415139198303</c:v>
+                  <c:v>0.04908329620957375</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.08195415139198303</c:v>
+                  <c:v>0.04619604349136353</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.08195415139198303</c:v>
+                  <c:v>0.04330879077315331</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.07740114629268646</c:v>
+                  <c:v>0.04330879077315331</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0728481337428093</c:v>
+                  <c:v>0.04042153805494309</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.06829512864351273</c:v>
+                  <c:v>0.04042153805494309</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.06829512864351273</c:v>
+                  <c:v>0.04042153805494309</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.06374211609363556</c:v>
+                  <c:v>0.04042153805494309</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.06374211609363556</c:v>
+                  <c:v>0.03753428533673286</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.06374211609363556</c:v>
+                  <c:v>0.02598527446389198</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.06374211609363556</c:v>
+                  <c:v>0.0144362635910511</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.05918911099433899</c:v>
+                  <c:v>0.01154901087284088</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.04097707569599152</c:v>
+                  <c:v>0.01154901087284088</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02276504226028919</c:v>
+                  <c:v>0.005774505436420441</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.01821203343570232</c:v>
+                  <c:v>0.005774505436420441</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.01821203343570232</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.009106016717851162</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.009106016717851162</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -706,8 +679,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H41" totalsRowCount="1">
-  <autoFilter ref="A2:H40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H38" totalsRowCount="1">
+  <autoFilter ref="A2:H37"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -723,8 +696,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H41" totalsRowCount="1">
-  <autoFilter ref="A2:H40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H38" totalsRowCount="1">
+  <autoFilter ref="A2:H37"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -1024,7 +997,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1040,28 +1013,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1069,25 +1042,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>92.76246643066406</v>
+        <v>86.59014129638672</v>
       </c>
       <c r="C3" s="1">
-        <v>13227</v>
+        <v>13276</v>
       </c>
       <c r="D3" s="1">
-        <v>37347</v>
+        <v>63482</v>
       </c>
       <c r="E3" s="1">
-        <v>37064</v>
+        <v>63216</v>
       </c>
       <c r="F3" s="1">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="G3" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1">
-        <v>13092</v>
+        <v>13140</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1095,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>7.181429386138916</v>
+        <v>13.3576831817627</v>
       </c>
       <c r="C4" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="D4" s="1">
         <v>404</v>
@@ -1113,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1121,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>0.02805245853960514</v>
+        <v>0.02608922496438026</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1147,7 +1120,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>0.02805245853960514</v>
+        <v>0.02608922496438026</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1168,35 +1141,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41">
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C38">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D41">
+      <c r="D38">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E41">
+      <c r="E38">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F41">
+      <c r="F38">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G41">
+      <c r="G38">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H41">
+      <c r="H38">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1212,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1228,28 +1201,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1257,25 +1230,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>85.02059936523438</v>
+        <v>91.644287109375</v>
       </c>
       <c r="C3" s="1">
-        <v>37347</v>
+        <v>63482</v>
       </c>
       <c r="D3" s="1">
-        <v>13227</v>
+        <v>13276</v>
       </c>
       <c r="E3" s="1">
-        <v>37064</v>
+        <v>63216</v>
       </c>
       <c r="F3" s="1">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="G3" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1">
-        <v>13092</v>
+        <v>13140</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1283,16 +1256,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>4.284380912780762</v>
+        <v>2.145228862762451</v>
       </c>
       <c r="C4" s="1">
-        <v>1882</v>
+        <v>1486</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>1882</v>
+        <v>1486</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1309,7 +1282,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>2.745464086532593</v>
+        <v>1.741013407707214</v>
       </c>
       <c r="C5" s="1">
         <v>1206</v>
@@ -1335,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>1.971452593803406</v>
+        <v>1.25018048286438</v>
       </c>
       <c r="C6" s="1">
         <v>866</v>
@@ -1361,13 +1334,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.919707715511322</v>
+        <v>0.5832250714302063</v>
       </c>
       <c r="C7" s="1">
         <v>404</v>
       </c>
       <c r="D7" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="E7" s="1">
         <v>36</v>
@@ -1379,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>1024</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1387,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>0.760352373123169</v>
+        <v>0.4821712076663971</v>
       </c>
       <c r="C8" s="1">
         <v>334</v>
@@ -1413,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0.51904296875</v>
+        <v>0.3291468024253845</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -1439,16 +1412,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>0.5053839087486267</v>
+        <v>0.2685145139694214</v>
       </c>
       <c r="C10" s="1">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1465,16 +1438,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.4234297871589661</v>
+        <v>0.2540782392024994</v>
       </c>
       <c r="C11" s="1">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1491,16 +1464,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>0.400664746761322</v>
+        <v>0.1587989032268524</v>
       </c>
       <c r="C12" s="1">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1517,16 +1490,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>0.282286524772644</v>
+        <v>0.1443626433610916</v>
       </c>
       <c r="C13" s="1">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1543,16 +1516,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>0.2504154741764069</v>
+        <v>0.08950483798980713</v>
       </c>
       <c r="C14" s="1">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1569,16 +1542,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>0.2276504188776016</v>
+        <v>0.07218132168054581</v>
       </c>
       <c r="C15" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1595,16 +1568,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.141143262386322</v>
+        <v>0.06351955980062485</v>
       </c>
       <c r="C16" s="1">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1621,16 +1594,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.1138252094388008</v>
+        <v>0.05774505436420441</v>
       </c>
       <c r="C17" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1647,16 +1620,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.1138252094388008</v>
+        <v>0.05197054892778397</v>
       </c>
       <c r="C18" s="1">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1673,16 +1646,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>0.1001661866903305</v>
+        <v>0.05197054892778397</v>
       </c>
       <c r="C19" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1699,16 +1672,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>0.09106016904115677</v>
+        <v>0.05197054892778397</v>
       </c>
       <c r="C20" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1725,7 +1698,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>0.08195415139198303</v>
+        <v>0.05197054892778397</v>
       </c>
       <c r="C21" s="1">
         <v>36</v>
@@ -1751,7 +1724,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.08195415139198303</v>
+        <v>0.05197054892778397</v>
       </c>
       <c r="C22" s="1">
         <v>36</v>
@@ -1777,16 +1750,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.08195415139198303</v>
+        <v>0.04908329620957375</v>
       </c>
       <c r="C23" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1803,16 +1776,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>0.08195415139198303</v>
+        <v>0.04619604349136353</v>
       </c>
       <c r="C24" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1829,16 +1802,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>0.08195415139198303</v>
+        <v>0.04330879077315331</v>
       </c>
       <c r="C25" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1855,16 +1828,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>0.07740114629268646</v>
+        <v>0.04330879077315331</v>
       </c>
       <c r="C26" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1881,16 +1854,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>0.0728481337428093</v>
+        <v>0.04042153805494309</v>
       </c>
       <c r="C27" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1907,16 +1880,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>0.06829512864351273</v>
+        <v>0.04042153805494309</v>
       </c>
       <c r="C28" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1933,16 +1906,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>0.06829512864351273</v>
+        <v>0.04042153805494309</v>
       </c>
       <c r="C29" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1959,7 +1932,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.06374211609363556</v>
+        <v>0.04042153805494309</v>
       </c>
       <c r="C30" s="1">
         <v>28</v>
@@ -1985,16 +1958,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.06374211609363556</v>
+        <v>0.03753428533673286</v>
       </c>
       <c r="C31" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2011,16 +1984,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.06374211609363556</v>
+        <v>0.02598527446389198</v>
       </c>
       <c r="C32" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2037,16 +2010,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.06374211609363556</v>
+        <v>0.0144362635910511</v>
       </c>
       <c r="C33" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2063,16 +2036,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>0.05918911099433899</v>
+        <v>0.01154901087284088</v>
       </c>
       <c r="C34" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2089,16 +2062,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>0.04097707569599152</v>
+        <v>0.01154901087284088</v>
       </c>
       <c r="C35" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2112,25 +2085,25 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="B36" s="2">
-        <v>0.02276504226028919</v>
+        <v>0.005774505436420441</v>
       </c>
       <c r="C36" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E36" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -2138,19 +2111,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
-        <v>0.01821203343570232</v>
+        <v>0.005774505436420441</v>
       </c>
       <c r="C37" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2163,112 +2136,34 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
-        <v>0.01821203343570232</v>
-      </c>
-      <c r="C38" s="1">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0</v>
-      </c>
-      <c r="E38" s="1">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0.009106016717851162</v>
-      </c>
-      <c r="C39" s="1">
-        <v>4</v>
-      </c>
-      <c r="D39" s="1">
-        <v>4</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1">
-        <v>4</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2">
-        <v>0.009106016717851162</v>
-      </c>
-      <c r="C40" s="1">
-        <v>4</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>4</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1">
-        <v>0</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41">
+      <c r="B38">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C38">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D41">
+      <c r="D38">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E41">
+      <c r="E38">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F41">
+      <c r="F38">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G41">
+      <c r="G38">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H41">
+      <c r="H38">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
change pid,fix ui error
</commit_message>
<xml_diff>
--- a/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
+++ b/app/project/MDK_V5/AT32F415RBT7_WorkBench_analysis.xlsx
@@ -15,35 +15,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>AT32F415RBT7_WorkBench</t>
   </si>
   <si>
-    <t>lto-llvm-132006.o</t>
+    <t>lto-llvm-db999c.o</t>
   </si>
   <si>
     <t>startup_at32f415.o</t>
   </si>
   <si>
+    <t>mf_w.l</t>
+  </si>
+  <si>
+    <t>dadd.o</t>
+  </si>
+  <si>
+    <t>dmul.o</t>
+  </si>
+  <si>
     <t>mc_w.l</t>
   </si>
   <si>
-    <t>stdout.o</t>
-  </si>
-  <si>
-    <t>mf_w.l</t>
-  </si>
-  <si>
-    <t>printf6.o</t>
-  </si>
-  <si>
-    <t>dadd.o</t>
-  </si>
-  <si>
-    <t>dmul.o</t>
-  </si>
-  <si>
     <t>depilogue.o</t>
   </si>
   <si>
@@ -62,19 +56,10 @@
     <t>dfixui.o</t>
   </si>
   <si>
-    <t>uidiv.o</t>
-  </si>
-  <si>
     <t>ffixui.o</t>
   </si>
   <si>
-    <t>puts.o</t>
-  </si>
-  <si>
     <t>memseta.o</t>
-  </si>
-  <si>
-    <t>memcpya.o</t>
   </si>
   <si>
     <t>llsshr.o</t>
@@ -242,22 +227,16 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ram_percent!$A$3:$A$38</c:f>
+              <c:f>ram_percent!$A$3:$A$33</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-132006.o</c:v>
+                  <c:v>lto-llvm-db999c.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>startup_at32f415.o</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>mc_w.l</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>stdout.o</c:v>
-                </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="30">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -265,23 +244,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ram_percent!$B$3:$B$38</c:f>
+              <c:f>ram_percent!$B$3:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>86.59014129638672</c:v>
+                  <c:v>92.83314514160156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.3576831817627</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.02608922496438026</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.02608922496438026</c:v>
-                </c:pt>
-                <c:pt idx="35">
+                  <c:v>7.166853427886963</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -349,115 +322,100 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>flash_percent!$A$3:$A$38</c:f>
+              <c:f>flash_percent!$A$3:$A$33</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>lto-llvm-132006.o</c:v>
+                  <c:v>lto-llvm-db999c.o</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>mf_w.l</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>startup_at32f415.o</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dadd.o</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dmul.o</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>mc_w.l</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>printf6.o</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>startup_at32f415.o</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dadd.o</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>dmul.o</c:v>
+                  <c:v>depilogue.o</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>depilogue.o</c:v>
+                  <c:v>fadd.o</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>fadd.o</c:v>
+                  <c:v>fepilogue.o</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>fepilogue.o</c:v>
+                  <c:v>fmul.o</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>fmul.o</c:v>
+                  <c:v>dfixi.o</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>dfixi.o</c:v>
+                  <c:v>dfixui.o</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>dfixui.o</c:v>
+                  <c:v>ffixui.o</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>uidiv.o</c:v>
+                  <c:v>memseta.o</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>ffixui.o</c:v>
+                  <c:v>llsshr.o</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>puts.o</c:v>
+                  <c:v>init.o</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>memseta.o</c:v>
+                  <c:v>dflti.o</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>memcpya.o</c:v>
+                  <c:v>llushr.o</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>llsshr.o</c:v>
+                  <c:v>llshl.o</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>init.o</c:v>
+                  <c:v>handlers.o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>dflti.o</c:v>
+                  <c:v>fcmplt.o</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>llushr.o</c:v>
+                  <c:v>fcmple.o</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>llshl.o</c:v>
+                  <c:v>fcmpgt.o</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>handlers.o</c:v>
+                  <c:v>fcmpge.o</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>fcmplt.o</c:v>
+                  <c:v>dfltui.o</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>fcmple.o</c:v>
+                  <c:v>fflti.o</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>fcmpgt.o</c:v>
+                  <c:v>ffltui.o</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>fcmpge.o</c:v>
+                  <c:v>entry9a.o</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>dfltui.o</c:v>
+                  <c:v>entry2.o</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>fflti.o</c:v>
+                  <c:v>entry5.o</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>ffltui.o</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>entry9a.o</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>entry2.o</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>stdout.o</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>entry5.o</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>Totals</c:v>
                 </c:pt>
               </c:strCache>
@@ -465,116 +423,101 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>flash_percent!$B$3:$B$38</c:f>
+              <c:f>flash_percent!$B$3:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>91.644287109375</c:v>
+                  <c:v>94.33794403076172</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.145228862762451</c:v>
+                  <c:v>2.204878568649292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.741013407707214</c:v>
+                  <c:v>0.5994421243667603</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.25018048286438</c:v>
+                  <c:v>0.4955783784389496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5832250714302063</c:v>
+                  <c:v>0.3382990062236786</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4821712076663971</c:v>
+                  <c:v>0.3264288604259491</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3291468024253845</c:v>
+                  <c:v>0.2759807705879211</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2685145139694214</c:v>
+                  <c:v>0.2611430883407593</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2540782392024994</c:v>
+                  <c:v>0.1632144302129746</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1587989032268524</c:v>
+                  <c:v>0.1483767628669739</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1443626433610916</c:v>
+                  <c:v>0.09199359267950058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08950483798980713</c:v>
+                  <c:v>0.07418838143348694</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.07218132168054581</c:v>
+                  <c:v>0.05935070291161537</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06351955980062485</c:v>
+                  <c:v>0.05341563373804092</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05774505436420441</c:v>
+                  <c:v>0.05341563373804092</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05197054892778397</c:v>
+                  <c:v>0.05341563373804092</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05197054892778397</c:v>
+                  <c:v>0.05044809728860855</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05197054892778397</c:v>
+                  <c:v>0.04748056083917618</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.05197054892778397</c:v>
+                  <c:v>0.0445130281150341</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.05197054892778397</c:v>
+                  <c:v>0.0445130281150341</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04908329620957375</c:v>
+                  <c:v>0.04154549166560173</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.04619604349136353</c:v>
+                  <c:v>0.04154549166560173</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.04330879077315331</c:v>
+                  <c:v>0.04154549166560173</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.04330879077315331</c:v>
+                  <c:v>0.04154549166560173</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.04042153805494309</c:v>
+                  <c:v>0.03857795894145966</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.04042153805494309</c:v>
+                  <c:v>0.02670781686902046</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.04042153805494309</c:v>
+                  <c:v>0.01483767572790384</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.04042153805494309</c:v>
+                  <c:v>0.01187014020979404</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03753428533673286</c:v>
+                  <c:v>0.01187014020979404</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.02598527446389198</c:v>
+                  <c:v>0.005935070104897022</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0144362635910511</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.01154901087284088</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.01154901087284088</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.005774505436420441</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.005774505436420441</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -679,8 +622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H38" totalsRowCount="1">
-  <autoFilter ref="A2:H37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H33" totalsRowCount="1">
+  <autoFilter ref="A2:H32"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="ram_percent" totalsRowFunction="sum"/>
@@ -696,8 +639,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H38" totalsRowCount="1">
-  <autoFilter ref="A2:H37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H33" totalsRowCount="1">
+  <autoFilter ref="A2:H32"/>
   <tableColumns count="8">
     <tableColumn id="1" name="File_name" totalsRowLabel="Totals"/>
     <tableColumn id="2" name="flash_percent" totalsRowFunction="sum"/>
@@ -997,7 +940,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1013,28 +956,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1042,25 +985,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>86.59014129638672</v>
+        <v>92.83314514160156</v>
       </c>
       <c r="C3" s="1">
-        <v>13276</v>
+        <v>13264</v>
       </c>
       <c r="D3" s="1">
-        <v>63482</v>
+        <v>63580</v>
       </c>
       <c r="E3" s="1">
-        <v>63216</v>
+        <v>63318</v>
       </c>
       <c r="F3" s="1">
         <v>130</v>
       </c>
       <c r="G3" s="1">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H3" s="1">
-        <v>13140</v>
+        <v>13132</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1068,10 +1011,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>13.3576831817627</v>
+        <v>7.166853427886963</v>
       </c>
       <c r="C4" s="1">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="D4" s="1">
         <v>404</v>
@@ -1086,90 +1029,38 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.02608922496438026</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1206</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1202</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.02608922496438026</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
         <f>SUBTOTAL(109,[ram_percent])</f>
         <v>0</v>
       </c>
-      <c r="C38">
+      <c r="C33">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="D38">
+      <c r="D33">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="E38">
+      <c r="E33">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F33">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G38">
+      <c r="G33">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H38">
+      <c r="H33">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>
@@ -1185,7 +1076,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1201,28 +1092,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1230,33 +1121,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>91.644287109375</v>
+        <v>94.33794403076172</v>
       </c>
       <c r="C3" s="1">
-        <v>63482</v>
+        <v>63580</v>
       </c>
       <c r="D3" s="1">
-        <v>13276</v>
+        <v>13264</v>
       </c>
       <c r="E3" s="1">
-        <v>63216</v>
+        <v>63318</v>
       </c>
       <c r="F3" s="1">
         <v>130</v>
       </c>
       <c r="G3" s="1">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H3" s="1">
-        <v>13140</v>
+        <v>13132</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.145228862762451</v>
+        <v>2.204878568649292</v>
       </c>
       <c r="C4" s="1">
         <v>1486</v>
@@ -1279,45 +1170,45 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>1.741013407707214</v>
+        <v>0.5994421243667603</v>
       </c>
       <c r="C5" s="1">
-        <v>1206</v>
+        <v>404</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>1024</v>
       </c>
       <c r="E5" s="1">
-        <v>1202</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="G5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>1.25018048286438</v>
+        <v>0.4955783784389496</v>
       </c>
       <c r="C6" s="1">
-        <v>866</v>
+        <v>334</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>866</v>
+        <v>334</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1331,45 +1222,45 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>0.5832250714302063</v>
+        <v>0.3382990062236786</v>
       </c>
       <c r="C7" s="1">
-        <v>404</v>
+        <v>228</v>
       </c>
       <c r="D7" s="1">
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>36</v>
+        <v>228</v>
       </c>
       <c r="F7" s="1">
-        <v>368</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>2048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>0.4821712076663971</v>
+        <v>0.3264288604259491</v>
       </c>
       <c r="C8" s="1">
-        <v>334</v>
+        <v>220</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>334</v>
+        <v>220</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1383,19 +1274,19 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>0.3291468024253845</v>
+        <v>0.2759807705879211</v>
       </c>
       <c r="C9" s="1">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1409,19 +1300,19 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2685145139694214</v>
+        <v>0.2611430883407593</v>
       </c>
       <c r="C10" s="1">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1435,19 +1326,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>0.2540782392024994</v>
+        <v>0.1632144302129746</v>
       </c>
       <c r="C11" s="1">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1461,19 +1352,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>0.1587989032268524</v>
+        <v>0.1483767628669739</v>
       </c>
       <c r="C12" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1487,19 +1378,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>0.1443626433610916</v>
+        <v>0.09199359267950058</v>
       </c>
       <c r="C13" s="1">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1513,19 +1404,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>0.08950483798980713</v>
+        <v>0.07418838143348694</v>
       </c>
       <c r="C14" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1539,19 +1430,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>0.07218132168054581</v>
+        <v>0.05935070291161537</v>
       </c>
       <c r="C15" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1565,19 +1456,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.06351955980062485</v>
+        <v>0.05341563373804092</v>
       </c>
       <c r="C16" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1591,19 +1482,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>0.05774505436420441</v>
+        <v>0.05341563373804092</v>
       </c>
       <c r="C17" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1617,10 +1508,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.05197054892778397</v>
+        <v>0.05341563373804092</v>
       </c>
       <c r="C18" s="1">
         <v>36</v>
@@ -1643,19 +1534,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>0.05197054892778397</v>
+        <v>0.05044809728860855</v>
       </c>
       <c r="C19" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1669,19 +1560,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>0.05197054892778397</v>
+        <v>0.04748056083917618</v>
       </c>
       <c r="C20" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1695,19 +1586,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>0.05197054892778397</v>
+        <v>0.0445130281150341</v>
       </c>
       <c r="C21" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1721,19 +1612,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>0.05197054892778397</v>
+        <v>0.0445130281150341</v>
       </c>
       <c r="C22" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1747,19 +1638,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04908329620957375</v>
+        <v>0.04154549166560173</v>
       </c>
       <c r="C23" s="1">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1773,19 +1664,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>0.04619604349136353</v>
+        <v>0.04154549166560173</v>
       </c>
       <c r="C24" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1799,19 +1690,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>0.04330879077315331</v>
+        <v>0.04154549166560173</v>
       </c>
       <c r="C25" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1825,19 +1716,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>0.04330879077315331</v>
+        <v>0.04154549166560173</v>
       </c>
       <c r="C26" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1851,19 +1742,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.03857795894145966</v>
+      </c>
+      <c r="C27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
-        <v>0.04042153805494309</v>
-      </c>
-      <c r="C27" s="1">
-        <v>28</v>
-      </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1877,19 +1768,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>0.04042153805494309</v>
+        <v>0.02670781686902046</v>
       </c>
       <c r="C28" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1903,19 +1794,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>0.04042153805494309</v>
+        <v>0.01483767572790384</v>
       </c>
       <c r="C29" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1929,19 +1820,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>0.04042153805494309</v>
+        <v>0.01187014020979404</v>
       </c>
       <c r="C30" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -1955,19 +1846,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>0.03753428533673286</v>
+        <v>0.01187014020979404</v>
       </c>
       <c r="C31" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -1981,19 +1872,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>0.02598527446389198</v>
+        <v>0.005935070104897022</v>
       </c>
       <c r="C32" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2006,164 +1897,34 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
-        <v>0.0144362635910511</v>
-      </c>
-      <c r="C33" s="1">
-        <v>10</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
-        <v>10</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.01154901087284088</v>
-      </c>
-      <c r="C34" s="1">
-        <v>8</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
-        <v>8</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.01154901087284088</v>
-      </c>
-      <c r="C35" s="1">
-        <v>8</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0.005774505436420441</v>
-      </c>
-      <c r="C36" s="1">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>4</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.005774505436420441</v>
-      </c>
-      <c r="C37" s="1">
-        <v>4</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>4</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
+      <c r="B33">
         <f>SUBTOTAL(109,[flash_percent])</f>
         <v>0</v>
       </c>
-      <c r="C38">
+      <c r="C33">
         <f>SUBTOTAL(109,[flash])</f>
         <v>0</v>
       </c>
-      <c r="D38">
+      <c r="D33">
         <f>SUBTOTAL(109,[ram])</f>
         <v>0</v>
       </c>
-      <c r="E38">
+      <c r="E33">
         <f>SUBTOTAL(109,[Code])</f>
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F33">
         <f>SUBTOTAL(109,[RO_data])</f>
         <v>0</v>
       </c>
-      <c r="G38">
+      <c r="G33">
         <f>SUBTOTAL(109,[RW_data])</f>
         <v>0</v>
       </c>
-      <c r="H38">
+      <c r="H33">
         <f>SUBTOTAL(109,[ZI_data])</f>
         <v>0</v>
       </c>

</xml_diff>